<commit_message>
completed ppt and cluster pathway identification
</commit_message>
<xml_diff>
--- a/pubmed cataract related genes/PubMed_ClusterONE.xlsx
+++ b/pubmed cataract related genes/PubMed_ClusterONE.xlsx
@@ -15,12 +15,12 @@
     <sheet name="PubMed_ClusterONE" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="312">
   <si>
     <t>TMCO3</t>
   </si>
@@ -935,6 +935,27 @@
   </si>
   <si>
     <t>G-quadruplex DNA unwinding</t>
+  </si>
+  <si>
+    <t>MAR2</t>
+  </si>
+  <si>
+    <t>regulation of metanephric glomerulus development</t>
+  </si>
+  <si>
+    <t>FDR</t>
+  </si>
+  <si>
+    <t>positive regulation of synaptic plasticity</t>
+  </si>
+  <si>
+    <t>regulation of Wnt signaling pathway, planar cell polarity pathway</t>
+  </si>
+  <si>
+    <t>&gt;0.05</t>
+  </si>
+  <si>
+    <t>regulation of synaptic vesicle fusion to presynaptic active zone membrane</t>
   </si>
 </sst>
 </file>
@@ -1420,7 +1441,6 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1428,6 +1448,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1752,7 +1773,7 @@
   <dimension ref="A1:AP53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1770,19 +1791,22 @@
       <c r="C1" t="s">
         <v>297</v>
       </c>
+      <c r="E1" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="2" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A2">
-        <f>COUNTA(F2:AP2)</f>
+        <f t="shared" ref="A2:A33" si="0">COUNTA(F2:AP2)</f>
         <v>37</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="3">
         <v>7.3287643592712104E-7</v>
       </c>
       <c r="C2" t="s">
         <v>298</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>2.01E-2</v>
       </c>
       <c r="F2" t="s">
@@ -1899,16 +1923,16 @@
     </row>
     <row r="3" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A3">
-        <f>COUNTA(F3:AP3)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>0.228959891043719</v>
       </c>
       <c r="C3" t="s">
         <v>299</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>3.3400000000000001E-3</v>
       </c>
       <c r="F3" t="s">
@@ -1938,16 +1962,16 @@
     </row>
     <row r="4" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f>COUNTA(F4:AP4)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>0.34817626635343701</v>
       </c>
       <c r="C4" t="s">
         <v>300</v>
       </c>
-      <c r="E4" s="3">
+      <c r="E4" s="2">
         <v>4.8300000000000001E-3</v>
       </c>
       <c r="F4" t="s">
@@ -1974,16 +1998,16 @@
     </row>
     <row r="5" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f>COUNTA(F5:AP5)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>0.34850384163236298</v>
       </c>
       <c r="C5" t="s">
         <v>301</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="2">
         <v>2.07E-2</v>
       </c>
       <c r="F5" t="s">
@@ -2010,10 +2034,10 @@
     </row>
     <row r="6" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f>COUNTA(F6:AP6)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>0.34931360216484098</v>
       </c>
       <c r="E6" t="s">
@@ -2043,10 +2067,10 @@
     </row>
     <row r="7" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f>COUNTA(F7:AP7)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>0.18011275326930801</v>
       </c>
       <c r="E7" t="s">
@@ -2073,10 +2097,10 @@
     </row>
     <row r="8" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f>COUNTA(F8:AP8)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>0.20753155345410601</v>
       </c>
       <c r="E8" t="s">
@@ -2103,16 +2127,16 @@
     </row>
     <row r="9" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A9">
-        <f>COUNTA(F9:AP9)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>0.18011275326930801</v>
       </c>
       <c r="C9" t="s">
         <v>303</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>6.62E-3</v>
       </c>
       <c r="F9" t="s">
@@ -2136,16 +2160,16 @@
     </row>
     <row r="10" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f>COUNTA(F10:AP10)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>0.179658669107819</v>
       </c>
       <c r="C10" t="s">
         <v>304</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>1.9300000000000001E-2</v>
       </c>
       <c r="F10" t="s">
@@ -2169,10 +2193,10 @@
     </row>
     <row r="11" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f>COUNTA(F11:AP11)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>0.18235566852621099</v>
       </c>
       <c r="E11" t="s">
@@ -2199,11 +2223,14 @@
     </row>
     <row r="12" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A12">
-        <f>COUNTA(F12:AP12)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>0.18235566852621099</v>
+      </c>
+      <c r="E12" t="s">
+        <v>302</v>
       </c>
       <c r="F12" t="s">
         <v>38</v>
@@ -2226,11 +2253,14 @@
     </row>
     <row r="13" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A13">
-        <f>COUNTA(F13:AP13)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>0.27871058240279001</v>
+      </c>
+      <c r="E13" t="s">
+        <v>302</v>
       </c>
       <c r="F13" t="s">
         <v>44</v>
@@ -2253,11 +2283,14 @@
     </row>
     <row r="14" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A14">
-        <f>COUNTA(F14:AP14)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>0.182798831597038</v>
+      </c>
+      <c r="E14" t="s">
+        <v>302</v>
       </c>
       <c r="F14" t="s">
         <v>14</v>
@@ -2280,11 +2313,14 @@
     </row>
     <row r="15" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A15">
-        <f>COUNTA(F15:AP15)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>0.53224616276680603</v>
+      </c>
+      <c r="E15" t="s">
+        <v>302</v>
       </c>
       <c r="F15" t="s">
         <v>114</v>
@@ -2307,11 +2343,14 @@
     </row>
     <row r="16" spans="1:42" x14ac:dyDescent="0.25">
       <c r="A16">
-        <f>COUNTA(F16:AP16)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>0.53241992789590598</v>
+      </c>
+      <c r="E16" t="s">
+        <v>302</v>
       </c>
       <c r="F16" t="s">
         <v>6</v>
@@ -2334,11 +2373,17 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17">
-        <f>COUNTA(F17:AP17)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>0.179658669107819</v>
+      </c>
+      <c r="C17" t="s">
+        <v>306</v>
+      </c>
+      <c r="E17" s="2">
+        <v>0.01</v>
       </c>
       <c r="F17" t="s">
         <v>152</v>
@@ -2361,11 +2406,14 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18">
-        <f>COUNTA(F18:AP18)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>0.45681333053791501</v>
+      </c>
+      <c r="E18" t="s">
+        <v>302</v>
       </c>
       <c r="F18" t="s">
         <v>50</v>
@@ -2385,11 +2433,14 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19">
-        <f>COUNTA(F19:AP19)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>0.33471120899742601</v>
+      </c>
+      <c r="E19" t="s">
+        <v>302</v>
       </c>
       <c r="F19" t="s">
         <v>109</v>
@@ -2409,11 +2460,14 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20">
-        <f>COUNTA(F20:AP20)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>0.33471120899742601</v>
+      </c>
+      <c r="E20" t="s">
+        <v>302</v>
       </c>
       <c r="F20" t="s">
         <v>120</v>
@@ -2433,11 +2487,17 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21">
-        <f>COUNTA(F21:AP21)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>0.33321501693390698</v>
+      </c>
+      <c r="C21" t="s">
+        <v>304</v>
+      </c>
+      <c r="E21" s="2">
+        <v>2.8700000000000002E-3</v>
       </c>
       <c r="F21" t="s">
         <v>26</v>
@@ -2457,11 +2517,17 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22">
-        <f>COUNTA(F22:AP22)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>0.33321501693390698</v>
+      </c>
+      <c r="C22" t="s">
+        <v>308</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1.4200000000000001E-2</v>
       </c>
       <c r="F22" t="s">
         <v>158</v>
@@ -2481,11 +2547,14 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23">
-        <f>COUNTA(F23:AP23)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>0.33321501693390698</v>
+      </c>
+      <c r="E23" t="s">
+        <v>302</v>
       </c>
       <c r="F23" t="s">
         <v>158</v>
@@ -2505,11 +2574,14 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24">
-        <f>COUNTA(F24:AP24)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>0.33321501693390698</v>
+      </c>
+      <c r="E24" t="s">
+        <v>302</v>
       </c>
       <c r="F24" t="s">
         <v>168</v>
@@ -2529,11 +2601,14 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25">
-        <f>COUNTA(F25:AP25)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>0.33471120899742601</v>
+      </c>
+      <c r="E25" t="s">
+        <v>302</v>
       </c>
       <c r="F25" t="s">
         <v>136</v>
@@ -2553,11 +2628,14 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26">
-        <f>COUNTA(F26:AP26)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>0.33321501693390698</v>
+      </c>
+      <c r="E26" t="s">
+        <v>302</v>
       </c>
       <c r="F26" t="s">
         <v>195</v>
@@ -2577,11 +2655,17 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27">
-        <f>COUNTA(F27:AP27)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>0.33471120899742601</v>
+      </c>
+      <c r="C27" t="s">
+        <v>309</v>
+      </c>
+      <c r="E27" s="2">
+        <v>2.86E-2</v>
       </c>
       <c r="F27" t="s">
         <v>152</v>
@@ -2601,11 +2685,14 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28">
-        <f>COUNTA(F28:AP28)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>0.45667206006378103</v>
+      </c>
+      <c r="E28" t="s">
+        <v>302</v>
       </c>
       <c r="F28" t="s">
         <v>214</v>
@@ -2625,11 +2712,14 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29">
-        <f>COUNTA(F29:AP29)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>0.33321501693390698</v>
+      </c>
+      <c r="E29" t="s">
+        <v>302</v>
       </c>
       <c r="F29" t="s">
         <v>222</v>
@@ -2649,11 +2739,14 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30">
-        <f>COUNTA(F30:AP30)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>0.33321501693390698</v>
+      </c>
+      <c r="E30" t="s">
+        <v>302</v>
       </c>
       <c r="F30" t="s">
         <v>120</v>
@@ -2673,11 +2766,14 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31">
-        <f>COUNTA(F31:AP31)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>0.33321501693390698</v>
+      </c>
+      <c r="E31" t="s">
+        <v>302</v>
       </c>
       <c r="F31" t="s">
         <v>218</v>
@@ -2697,11 +2793,14 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32">
-        <f>COUNTA(F32:AP32)</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B32" s="2">
+      <c r="B32" s="1">
         <v>0.33321501693390698</v>
+      </c>
+      <c r="E32" t="s">
+        <v>302</v>
       </c>
       <c r="F32" t="s">
         <v>238</v>
@@ -2721,11 +2820,14 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <f>COUNTA(F33:AP33)</f>
-        <v>4</v>
-      </c>
-      <c r="B33" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B33" s="1">
         <v>0.561522678679932</v>
+      </c>
+      <c r="E33" t="s">
+        <v>302</v>
       </c>
       <c r="F33" t="s">
         <v>55</v>
@@ -2742,11 +2844,14 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <f>COUNTA(F34:AP34)</f>
-        <v>4</v>
-      </c>
-      <c r="B34" s="2">
+        <f t="shared" ref="A34:A53" si="1">COUNTA(F34:AP34)</f>
+        <v>4</v>
+      </c>
+      <c r="B34" s="1">
         <v>0.561522678679932</v>
+      </c>
+      <c r="E34" t="s">
+        <v>302</v>
       </c>
       <c r="F34" t="s">
         <v>101</v>
@@ -2763,11 +2868,14 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <f>COUNTA(F35:AP35)</f>
-        <v>4</v>
-      </c>
-      <c r="B35" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B35" s="1">
         <v>0.561522678679932</v>
+      </c>
+      <c r="E35" t="s">
+        <v>302</v>
       </c>
       <c r="F35" t="s">
         <v>105</v>
@@ -2784,17 +2892,20 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <f>COUNTA(F36:AP36)</f>
-        <v>4</v>
-      </c>
-      <c r="B36" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B36" s="1">
         <v>0.56194501973717004</v>
+      </c>
+      <c r="E36" t="s">
+        <v>302</v>
       </c>
       <c r="F36" t="s">
         <v>125</v>
       </c>
-      <c r="G36" s="1">
-        <v>43526</v>
+      <c r="G36" s="4" t="s">
+        <v>305</v>
       </c>
       <c r="H36" t="s">
         <v>126</v>
@@ -2805,11 +2916,14 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <f>COUNTA(F37:AP37)</f>
-        <v>4</v>
-      </c>
-      <c r="B37" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B37" s="1">
         <v>0.32227608523573797</v>
+      </c>
+      <c r="E37" t="s">
+        <v>310</v>
       </c>
       <c r="F37" t="s">
         <v>132</v>
@@ -2826,11 +2940,14 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <f>COUNTA(F38:AP38)</f>
-        <v>4</v>
-      </c>
-      <c r="B38" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B38" s="1">
         <v>0.561522678679932</v>
+      </c>
+      <c r="E38" t="s">
+        <v>310</v>
       </c>
       <c r="F38" t="s">
         <v>109</v>
@@ -2847,11 +2964,14 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <f>COUNTA(F39:AP39)</f>
-        <v>4</v>
-      </c>
-      <c r="B39" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B39" s="1">
         <v>0.561522678679932</v>
+      </c>
+      <c r="E39" t="s">
+        <v>310</v>
       </c>
       <c r="F39" t="s">
         <v>139</v>
@@ -2868,11 +2988,14 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <f>COUNTA(F40:AP40)</f>
-        <v>4</v>
-      </c>
-      <c r="B40" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B40" s="1">
         <v>0.561522678679932</v>
+      </c>
+      <c r="E40" t="s">
+        <v>310</v>
       </c>
       <c r="F40" t="s">
         <v>139</v>
@@ -2889,11 +3012,14 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <f>COUNTA(F41:AP41)</f>
-        <v>4</v>
-      </c>
-      <c r="B41" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B41" s="1">
         <v>0.56194501973717004</v>
+      </c>
+      <c r="E41" t="s">
+        <v>310</v>
       </c>
       <c r="F41" t="s">
         <v>145</v>
@@ -2910,11 +3036,14 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <f>COUNTA(F42:AP42)</f>
-        <v>4</v>
-      </c>
-      <c r="B42" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B42" s="1">
         <v>0.5</v>
+      </c>
+      <c r="E42" t="s">
+        <v>310</v>
       </c>
       <c r="F42" t="s">
         <v>154</v>
@@ -2931,11 +3060,17 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <f>COUNTA(F43:AP43)</f>
-        <v>4</v>
-      </c>
-      <c r="B43" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B43" s="1">
         <v>0.56194501973717004</v>
+      </c>
+      <c r="C43" t="s">
+        <v>311</v>
+      </c>
+      <c r="E43" s="2">
+        <v>1.4200000000000001E-2</v>
       </c>
       <c r="F43" t="s">
         <v>158</v>
@@ -2952,11 +3087,14 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <f>COUNTA(F44:AP44)</f>
-        <v>4</v>
-      </c>
-      <c r="B44" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B44" s="1">
         <v>0.56194501973717004</v>
+      </c>
+      <c r="E44" t="s">
+        <v>310</v>
       </c>
       <c r="F44" t="s">
         <v>175</v>
@@ -2973,11 +3111,14 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <f>COUNTA(F45:AP45)</f>
-        <v>4</v>
-      </c>
-      <c r="B45" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B45" s="1">
         <v>0.561522678679932</v>
+      </c>
+      <c r="E45" t="s">
+        <v>310</v>
       </c>
       <c r="F45" t="s">
         <v>179</v>
@@ -2994,11 +3135,14 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <f>COUNTA(F46:AP46)</f>
-        <v>4</v>
-      </c>
-      <c r="B46" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B46" s="1">
         <v>0.56194501973717004</v>
+      </c>
+      <c r="E46" t="s">
+        <v>310</v>
       </c>
       <c r="F46" t="s">
         <v>183</v>
@@ -3015,11 +3159,14 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <f>COUNTA(F47:AP47)</f>
-        <v>4</v>
-      </c>
-      <c r="B47" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B47" s="1">
         <v>0.5</v>
+      </c>
+      <c r="E47" t="s">
+        <v>310</v>
       </c>
       <c r="F47" t="s">
         <v>189</v>
@@ -3036,11 +3183,14 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <f>COUNTA(F48:AP48)</f>
-        <v>4</v>
-      </c>
-      <c r="B48" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B48" s="1">
         <v>0.561522678679932</v>
+      </c>
+      <c r="E48" t="s">
+        <v>310</v>
       </c>
       <c r="F48" t="s">
         <v>193</v>
@@ -3057,11 +3207,14 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <f>COUNTA(F49:AP49)</f>
-        <v>4</v>
-      </c>
-      <c r="B49" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B49" s="1">
         <v>0.5</v>
+      </c>
+      <c r="E49" t="s">
+        <v>310</v>
       </c>
       <c r="F49" t="s">
         <v>189</v>
@@ -3078,11 +3231,14 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <f>COUNTA(F50:AP50)</f>
-        <v>4</v>
-      </c>
-      <c r="B50" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B50" s="1">
         <v>0.56194501973717004</v>
+      </c>
+      <c r="E50" t="s">
+        <v>310</v>
       </c>
       <c r="F50" t="s">
         <v>210</v>
@@ -3099,11 +3255,14 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <f>COUNTA(F51:AP51)</f>
-        <v>4</v>
-      </c>
-      <c r="B51" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B51" s="1">
         <v>0.56194501973717004</v>
+      </c>
+      <c r="E51" t="s">
+        <v>310</v>
       </c>
       <c r="F51" t="s">
         <v>215</v>
@@ -3120,11 +3279,14 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <f>COUNTA(F52:AP52)</f>
-        <v>4</v>
-      </c>
-      <c r="B52" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B52" s="1">
         <v>0.79767161902456696</v>
+      </c>
+      <c r="E52" t="s">
+        <v>310</v>
       </c>
       <c r="F52" t="s">
         <v>48</v>
@@ -3141,11 +3303,14 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <f>COUNTA(F53:AP53)</f>
-        <v>4</v>
-      </c>
-      <c r="B53" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="B53" s="1">
         <v>0.561522678679932</v>
+      </c>
+      <c r="E53" t="s">
+        <v>310</v>
       </c>
       <c r="F53" t="s">
         <v>231</v>
@@ -3180,1198 +3345,1198 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="2">
+      <c r="B1" s="1">
         <v>37</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C1" s="1">
         <v>0.51951951951951902</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1" s="1">
         <v>346</v>
       </c>
-      <c r="E1" s="2">
+      <c r="E1" s="1">
         <v>197</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F1" s="1">
         <v>0.63720073664825005</v>
       </c>
-      <c r="G1" s="4">
+      <c r="G1" s="3">
         <v>7.3287643592712104E-7</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="1">
         <v>8</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="1">
         <v>0.67857142857142805</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2" s="1">
         <v>19</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="1">
         <v>105</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>0.15322580645161199</v>
       </c>
-      <c r="G2" s="2">
+      <c r="G2" s="1">
         <v>0.228959891043719</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="1">
         <v>7</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="1">
         <v>14</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="1">
         <v>105</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>0.11764705882352899</v>
       </c>
-      <c r="G3" s="2">
+      <c r="G3" s="1">
         <v>0.34817626635343701</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="1">
         <v>7</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="1">
         <v>0.61904761904761896</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <v>13</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="1">
         <v>105</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>0.11016949152542301</v>
       </c>
-      <c r="G4" s="2">
+      <c r="G4" s="1">
         <v>0.34850384163236298</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="1">
         <v>7</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <v>0.61904761904761896</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <v>13</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="1">
         <v>104</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>0.11111111111111099</v>
       </c>
-      <c r="G5" s="2">
+      <c r="G5" s="1">
         <v>0.34931360216484098</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="1">
         <v>6</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <v>10</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="1">
         <v>71</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>0.12345679012345601</v>
       </c>
-      <c r="G6" s="2">
+      <c r="G6" s="1">
         <v>0.18011275326930801</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="1">
         <v>6</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <v>0.6</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <v>9</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="1">
         <v>71</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="1">
         <v>0.1125</v>
       </c>
-      <c r="G7" s="2">
+      <c r="G7" s="1">
         <v>0.20753155345410601</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8" s="1">
         <v>6</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <v>10</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="1">
         <v>68</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="1">
         <v>0.128205128205128</v>
       </c>
-      <c r="G8" s="2">
+      <c r="G8" s="1">
         <v>0.18011275326930801</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9" s="1">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <v>10</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="1">
         <v>68</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>0.128205128205128</v>
       </c>
-      <c r="G9" s="2">
+      <c r="G9" s="1">
         <v>0.179658669107819</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="B10" s="2">
+      <c r="B10" s="1">
         <v>6</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="1">
         <v>10</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="1">
         <v>71</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>0.12345679012345601</v>
       </c>
-      <c r="G10" s="2">
+      <c r="G10" s="1">
         <v>0.18235566852621099</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="B11" s="2">
+      <c r="B11" s="1">
         <v>6</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="1">
         <v>10</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="1">
         <v>69</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>0.126582278481012</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G11" s="1">
         <v>0.18235566852621099</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B12" s="2">
+      <c r="B12" s="1">
         <v>6</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="1">
         <v>10</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="1">
         <v>72</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>0.12195121951219499</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G12" s="1">
         <v>0.27871058240279001</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B13" s="2">
+      <c r="B13" s="1">
         <v>6</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="1">
         <v>10</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="1">
         <v>70</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>0.125</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G13" s="1">
         <v>0.182798831597038</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B14" s="2">
+      <c r="B14" s="1">
         <v>6</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="1">
         <v>0.6</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="1">
         <v>9</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="1">
         <v>108</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="1">
         <v>7.69230769230769E-2</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G14" s="1">
         <v>0.53224616276680603</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B15" s="2">
+      <c r="B15" s="1">
         <v>6</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="1">
         <v>0.6</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="1">
         <v>9</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="1">
         <v>108</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="1">
         <v>7.69230769230769E-2</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G15" s="1">
         <v>0.53241992789590598</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="B16" s="2">
+      <c r="B16" s="1">
         <v>6</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="1">
         <v>0.6</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="1">
         <v>9</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="1">
         <v>70</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>0.113924050632911</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G16" s="1">
         <v>0.179658669107819</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="B17" s="2">
+      <c r="B17" s="1">
         <v>5</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="1">
         <v>0.6</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="1">
         <v>6</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="1">
         <v>75</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>7.4074074074074001E-2</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="1">
         <v>0.45681333053791501</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="B18" s="2">
+      <c r="B18" s="1">
         <v>5</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="1">
         <v>0.6</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="1">
         <v>6</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="1">
         <v>67</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>8.2191780821917804E-2</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="1">
         <v>0.33471120899742601</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>263</v>
       </c>
-      <c r="B19" s="2">
+      <c r="B19" s="1">
         <v>5</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="1">
         <v>0.6</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="1">
         <v>6</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="1">
         <v>72</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>7.69230769230769E-2</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="1">
         <v>0.33471120899742601</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="B20" s="2">
+      <c r="B20" s="1">
         <v>5</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="1">
         <v>0.6</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="1">
         <v>6</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="1">
         <v>74</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G20" s="1">
         <v>0.33321501693390698</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="B21" s="2">
+      <c r="B21" s="1">
         <v>5</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="1">
         <v>0.6</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="1">
         <v>6</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="1">
         <v>72</v>
       </c>
-      <c r="F21" s="2">
+      <c r="F21" s="1">
         <v>7.69230769230769E-2</v>
       </c>
-      <c r="G21" s="2">
+      <c r="G21" s="1">
         <v>0.33321501693390698</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="B22" s="2">
+      <c r="B22" s="1">
         <v>5</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="1">
         <v>0.6</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="1">
         <v>6</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="1">
         <v>72</v>
       </c>
-      <c r="F22" s="2">
+      <c r="F22" s="1">
         <v>7.69230769230769E-2</v>
       </c>
-      <c r="G22" s="2">
+      <c r="G22" s="1">
         <v>0.33321501693390698</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="B23" s="2">
+      <c r="B23" s="1">
         <v>5</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="1">
         <v>0.6</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="1">
         <v>6</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="1">
         <v>72</v>
       </c>
-      <c r="F23" s="2">
+      <c r="F23" s="1">
         <v>7.69230769230769E-2</v>
       </c>
-      <c r="G23" s="2">
+      <c r="G23" s="1">
         <v>0.33321501693390698</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="B24" s="2">
+      <c r="B24" s="1">
         <v>5</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="1">
         <v>0.6</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="1">
         <v>6</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="1">
         <v>67</v>
       </c>
-      <c r="F24" s="2">
+      <c r="F24" s="1">
         <v>8.2191780821917804E-2</v>
       </c>
-      <c r="G24" s="2">
+      <c r="G24" s="1">
         <v>0.33471120899742601</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="B25" s="2">
+      <c r="B25" s="1">
         <v>5</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="1">
         <v>0.6</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="1">
         <v>6</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="1">
         <v>72</v>
       </c>
-      <c r="F25" s="2">
+      <c r="F25" s="1">
         <v>7.69230769230769E-2</v>
       </c>
-      <c r="G25" s="2">
+      <c r="G25" s="1">
         <v>0.33321501693390698</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="B26" s="2">
+      <c r="B26" s="1">
         <v>5</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="1">
         <v>0.6</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="1">
         <v>6</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="1">
         <v>75</v>
       </c>
-      <c r="F26" s="2">
+      <c r="F26" s="1">
         <v>7.4074074074074001E-2</v>
       </c>
-      <c r="G26" s="2">
+      <c r="G26" s="1">
         <v>0.33471120899742601</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>271</v>
       </c>
-      <c r="B27" s="2">
+      <c r="B27" s="1">
         <v>5</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="1">
         <v>0.6</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="1">
         <v>6</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="1">
         <v>74</v>
       </c>
-      <c r="F27" s="2">
+      <c r="F27" s="1">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="G27" s="2">
+      <c r="G27" s="1">
         <v>0.45667206006378103</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="B28" s="2">
+      <c r="B28" s="1">
         <v>5</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="1">
         <v>0.6</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="1">
         <v>6</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="1">
         <v>72</v>
       </c>
-      <c r="F28" s="2">
+      <c r="F28" s="1">
         <v>7.69230769230769E-2</v>
       </c>
-      <c r="G28" s="2">
+      <c r="G28" s="1">
         <v>0.33321501693390698</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>273</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B29" s="1">
         <v>5</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="1">
         <v>0.6</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="1">
         <v>6</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="1">
         <v>70</v>
       </c>
-      <c r="F29" s="2">
+      <c r="F29" s="1">
         <v>7.8947368421052599E-2</v>
       </c>
-      <c r="G29" s="2">
+      <c r="G29" s="1">
         <v>0.33321501693390698</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="B30" s="2">
+      <c r="B30" s="1">
         <v>5</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="1">
         <v>0.6</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="1">
         <v>6</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="1">
         <v>72</v>
       </c>
-      <c r="F30" s="2">
+      <c r="F30" s="1">
         <v>7.69230769230769E-2</v>
       </c>
-      <c r="G30" s="2">
+      <c r="G30" s="1">
         <v>0.33321501693390698</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>275</v>
       </c>
-      <c r="B31" s="2">
+      <c r="B31" s="1">
         <v>5</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="1">
         <v>0.6</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="1">
         <v>6</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="1">
         <v>70</v>
       </c>
-      <c r="F31" s="2">
+      <c r="F31" s="1">
         <v>7.8947368421052599E-2</v>
       </c>
-      <c r="G31" s="2">
+      <c r="G31" s="1">
         <v>0.33321501693390698</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="B32" s="2">
-        <v>4</v>
-      </c>
-      <c r="C32" s="2">
+      <c r="B32" s="1">
+        <v>4</v>
+      </c>
+      <c r="C32" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D32" s="2">
-        <v>4</v>
-      </c>
-      <c r="E32" s="2">
+      <c r="D32" s="1">
+        <v>4</v>
+      </c>
+      <c r="E32" s="1">
         <v>75</v>
       </c>
-      <c r="F32" s="2">
+      <c r="F32" s="1">
         <v>5.0632911392405E-2</v>
       </c>
-      <c r="G32" s="2">
+      <c r="G32" s="1">
         <v>0.561522678679932</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A33" s="2" t="s">
+      <c r="A33" s="1" t="s">
         <v>277</v>
       </c>
-      <c r="B33" s="2">
-        <v>4</v>
-      </c>
-      <c r="C33" s="2">
+      <c r="B33" s="1">
+        <v>4</v>
+      </c>
+      <c r="C33" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D33" s="2">
-        <v>4</v>
-      </c>
-      <c r="E33" s="2">
+      <c r="D33" s="1">
+        <v>4</v>
+      </c>
+      <c r="E33" s="1">
         <v>75</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F33" s="1">
         <v>5.0632911392405E-2</v>
       </c>
-      <c r="G33" s="2">
+      <c r="G33" s="1">
         <v>0.561522678679932</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
+      <c r="A34" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B34" s="2">
-        <v>4</v>
-      </c>
-      <c r="C34" s="2">
+      <c r="B34" s="1">
+        <v>4</v>
+      </c>
+      <c r="C34" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D34" s="2">
-        <v>4</v>
-      </c>
-      <c r="E34" s="2">
+      <c r="D34" s="1">
+        <v>4</v>
+      </c>
+      <c r="E34" s="1">
         <v>75</v>
       </c>
-      <c r="F34" s="2">
+      <c r="F34" s="1">
         <v>5.0632911392405E-2</v>
       </c>
-      <c r="G34" s="2">
+      <c r="G34" s="1">
         <v>0.561522678679932</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="2" t="s">
+      <c r="A35" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="B35" s="2">
-        <v>4</v>
-      </c>
-      <c r="C35" s="2">
+      <c r="B35" s="1">
+        <v>4</v>
+      </c>
+      <c r="C35" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D35" s="2">
-        <v>4</v>
-      </c>
-      <c r="E35" s="2">
+      <c r="D35" s="1">
+        <v>4</v>
+      </c>
+      <c r="E35" s="1">
         <v>74</v>
       </c>
-      <c r="F35" s="2">
+      <c r="F35" s="1">
         <v>5.1282051282051197E-2</v>
       </c>
-      <c r="G35" s="2">
+      <c r="G35" s="1">
         <v>0.56194501973717004</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+      <c r="A36" s="1" t="s">
         <v>280</v>
       </c>
-      <c r="B36" s="2">
-        <v>4</v>
-      </c>
-      <c r="C36" s="2">
+      <c r="B36" s="1">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D36" s="2">
-        <v>4</v>
-      </c>
-      <c r="E36" s="2">
+      <c r="D36" s="1">
+        <v>4</v>
+      </c>
+      <c r="E36" s="1">
         <v>37</v>
       </c>
-      <c r="F36" s="2">
+      <c r="F36" s="1">
         <v>9.7560975609756101E-2</v>
       </c>
-      <c r="G36" s="2">
+      <c r="G36" s="1">
         <v>0.32227608523573797</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="B37" s="2">
-        <v>4</v>
-      </c>
-      <c r="C37" s="2">
+      <c r="B37" s="1">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D37" s="2">
-        <v>4</v>
-      </c>
-      <c r="E37" s="2">
+      <c r="D37" s="1">
+        <v>4</v>
+      </c>
+      <c r="E37" s="1">
         <v>69</v>
       </c>
-      <c r="F37" s="2">
+      <c r="F37" s="1">
         <v>5.4794520547945202E-2</v>
       </c>
-      <c r="G37" s="2">
+      <c r="G37" s="1">
         <v>0.561522678679932</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>282</v>
       </c>
-      <c r="B38" s="2">
-        <v>4</v>
-      </c>
-      <c r="C38" s="2">
+      <c r="B38" s="1">
+        <v>4</v>
+      </c>
+      <c r="C38" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D38" s="2">
-        <v>4</v>
-      </c>
-      <c r="E38" s="2">
+      <c r="D38" s="1">
+        <v>4</v>
+      </c>
+      <c r="E38" s="1">
         <v>75</v>
       </c>
-      <c r="F38" s="2">
+      <c r="F38" s="1">
         <v>5.0632911392405E-2</v>
       </c>
-      <c r="G38" s="2">
+      <c r="G38" s="1">
         <v>0.561522678679932</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="B39" s="2">
-        <v>4</v>
-      </c>
-      <c r="C39" s="2">
+      <c r="B39" s="1">
+        <v>4</v>
+      </c>
+      <c r="C39" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D39" s="2">
-        <v>4</v>
-      </c>
-      <c r="E39" s="2">
+      <c r="D39" s="1">
+        <v>4</v>
+      </c>
+      <c r="E39" s="1">
         <v>75</v>
       </c>
-      <c r="F39" s="2">
+      <c r="F39" s="1">
         <v>5.0632911392405E-2</v>
       </c>
-      <c r="G39" s="2">
+      <c r="G39" s="1">
         <v>0.561522678679932</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="B40" s="2">
-        <v>4</v>
-      </c>
-      <c r="C40" s="2">
+      <c r="B40" s="1">
+        <v>4</v>
+      </c>
+      <c r="C40" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D40" s="2">
-        <v>4</v>
-      </c>
-      <c r="E40" s="2">
+      <c r="D40" s="1">
+        <v>4</v>
+      </c>
+      <c r="E40" s="1">
         <v>74</v>
       </c>
-      <c r="F40" s="2">
+      <c r="F40" s="1">
         <v>5.1282051282051197E-2</v>
       </c>
-      <c r="G40" s="2">
+      <c r="G40" s="1">
         <v>0.56194501973717004</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="B41" s="2">
-        <v>4</v>
-      </c>
-      <c r="C41" s="2">
+      <c r="B41" s="1">
+        <v>4</v>
+      </c>
+      <c r="C41" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D41" s="2">
-        <v>4</v>
-      </c>
-      <c r="E41" s="2">
+      <c r="D41" s="1">
+        <v>4</v>
+      </c>
+      <c r="E41" s="1">
         <v>39</v>
       </c>
-      <c r="F41" s="2">
+      <c r="F41" s="1">
         <v>9.3023255813953404E-2</v>
       </c>
-      <c r="G41" s="2">
+      <c r="G41" s="1">
         <v>0.5</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="2" t="s">
+      <c r="A42" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="B42" s="2">
-        <v>4</v>
-      </c>
-      <c r="C42" s="2">
+      <c r="B42" s="1">
+        <v>4</v>
+      </c>
+      <c r="C42" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D42" s="2">
-        <v>4</v>
-      </c>
-      <c r="E42" s="2">
+      <c r="D42" s="1">
+        <v>4</v>
+      </c>
+      <c r="E42" s="1">
         <v>74</v>
       </c>
-      <c r="F42" s="2">
+      <c r="F42" s="1">
         <v>5.1282051282051197E-2</v>
       </c>
-      <c r="G42" s="2">
+      <c r="G42" s="1">
         <v>0.56194501973717004</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B43" s="2">
-        <v>4</v>
-      </c>
-      <c r="C43" s="2">
+      <c r="B43" s="1">
+        <v>4</v>
+      </c>
+      <c r="C43" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D43" s="2">
-        <v>4</v>
-      </c>
-      <c r="E43" s="2">
+      <c r="D43" s="1">
+        <v>4</v>
+      </c>
+      <c r="E43" s="1">
         <v>74</v>
       </c>
-      <c r="F43" s="2">
+      <c r="F43" s="1">
         <v>5.1282051282051197E-2</v>
       </c>
-      <c r="G43" s="2">
+      <c r="G43" s="1">
         <v>0.56194501973717004</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="B44" s="2">
-        <v>4</v>
-      </c>
-      <c r="C44" s="2">
+      <c r="B44" s="1">
+        <v>4</v>
+      </c>
+      <c r="C44" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D44" s="2">
-        <v>4</v>
-      </c>
-      <c r="E44" s="2">
+      <c r="D44" s="1">
+        <v>4</v>
+      </c>
+      <c r="E44" s="1">
         <v>75</v>
       </c>
-      <c r="F44" s="2">
+      <c r="F44" s="1">
         <v>5.0632911392405E-2</v>
       </c>
-      <c r="G44" s="2">
+      <c r="G44" s="1">
         <v>0.561522678679932</v>
       </c>
     </row>
     <row r="45" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A45" s="2" t="s">
+      <c r="A45" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="B45" s="2">
-        <v>4</v>
-      </c>
-      <c r="C45" s="2">
+      <c r="B45" s="1">
+        <v>4</v>
+      </c>
+      <c r="C45" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D45" s="2">
-        <v>4</v>
-      </c>
-      <c r="E45" s="2">
+      <c r="D45" s="1">
+        <v>4</v>
+      </c>
+      <c r="E45" s="1">
         <v>74</v>
       </c>
-      <c r="F45" s="2">
+      <c r="F45" s="1">
         <v>5.1282051282051197E-2</v>
       </c>
-      <c r="G45" s="2">
+      <c r="G45" s="1">
         <v>0.56194501973717004</v>
       </c>
     </row>
     <row r="46" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>290</v>
       </c>
-      <c r="B46" s="2">
-        <v>4</v>
-      </c>
-      <c r="C46" s="2">
+      <c r="B46" s="1">
+        <v>4</v>
+      </c>
+      <c r="C46" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D46" s="2">
-        <v>4</v>
-      </c>
-      <c r="E46" s="2">
+      <c r="D46" s="1">
+        <v>4</v>
+      </c>
+      <c r="E46" s="1">
         <v>38</v>
       </c>
-      <c r="F46" s="2">
+      <c r="F46" s="1">
         <v>9.5238095238095205E-2</v>
       </c>
-      <c r="G46" s="2">
+      <c r="G46" s="1">
         <v>0.5</v>
       </c>
     </row>
     <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="2" t="s">
+      <c r="A47" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="B47" s="2">
-        <v>4</v>
-      </c>
-      <c r="C47" s="2">
+      <c r="B47" s="1">
+        <v>4</v>
+      </c>
+      <c r="C47" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D47" s="2">
-        <v>4</v>
-      </c>
-      <c r="E47" s="2">
+      <c r="D47" s="1">
+        <v>4</v>
+      </c>
+      <c r="E47" s="1">
         <v>75</v>
       </c>
-      <c r="F47" s="2">
+      <c r="F47" s="1">
         <v>5.0632911392405E-2</v>
       </c>
-      <c r="G47" s="2">
+      <c r="G47" s="1">
         <v>0.561522678679932</v>
       </c>
     </row>
     <row r="48" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A48" s="2" t="s">
+      <c r="A48" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B48" s="2">
-        <v>4</v>
-      </c>
-      <c r="C48" s="2">
+      <c r="B48" s="1">
+        <v>4</v>
+      </c>
+      <c r="C48" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D48" s="2">
-        <v>4</v>
-      </c>
-      <c r="E48" s="2">
+      <c r="D48" s="1">
+        <v>4</v>
+      </c>
+      <c r="E48" s="1">
         <v>38</v>
       </c>
-      <c r="F48" s="2">
+      <c r="F48" s="1">
         <v>9.5238095238095205E-2</v>
       </c>
-      <c r="G48" s="2">
+      <c r="G48" s="1">
         <v>0.5</v>
       </c>
     </row>
     <row r="49" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>293</v>
       </c>
-      <c r="B49" s="2">
-        <v>4</v>
-      </c>
-      <c r="C49" s="2">
+      <c r="B49" s="1">
+        <v>4</v>
+      </c>
+      <c r="C49" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D49" s="2">
-        <v>4</v>
-      </c>
-      <c r="E49" s="2">
+      <c r="D49" s="1">
+        <v>4</v>
+      </c>
+      <c r="E49" s="1">
         <v>74</v>
       </c>
-      <c r="F49" s="2">
+      <c r="F49" s="1">
         <v>5.1282051282051197E-2</v>
       </c>
-      <c r="G49" s="2">
+      <c r="G49" s="1">
         <v>0.56194501973717004</v>
       </c>
     </row>
     <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>294</v>
       </c>
-      <c r="B50" s="2">
-        <v>4</v>
-      </c>
-      <c r="C50" s="2">
+      <c r="B50" s="1">
+        <v>4</v>
+      </c>
+      <c r="C50" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D50" s="2">
-        <v>4</v>
-      </c>
-      <c r="E50" s="2">
+      <c r="D50" s="1">
+        <v>4</v>
+      </c>
+      <c r="E50" s="1">
         <v>74</v>
       </c>
-      <c r="F50" s="2">
+      <c r="F50" s="1">
         <v>5.1282051282051197E-2</v>
       </c>
-      <c r="G50" s="2">
+      <c r="G50" s="1">
         <v>0.56194501973717004</v>
       </c>
     </row>
     <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="B51" s="2">
-        <v>4</v>
-      </c>
-      <c r="C51" s="2">
+      <c r="B51" s="1">
+        <v>4</v>
+      </c>
+      <c r="C51" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D51" s="2">
-        <v>4</v>
-      </c>
-      <c r="E51" s="2">
+      <c r="D51" s="1">
+        <v>4</v>
+      </c>
+      <c r="E51" s="1">
         <v>76</v>
       </c>
-      <c r="F51" s="2">
+      <c r="F51" s="1">
         <v>0.05</v>
       </c>
-      <c r="G51" s="2">
+      <c r="G51" s="1">
         <v>0.79767161902456696</v>
       </c>
     </row>
     <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>296</v>
       </c>
-      <c r="B52" s="2">
-        <v>4</v>
-      </c>
-      <c r="C52" s="2">
+      <c r="B52" s="1">
+        <v>4</v>
+      </c>
+      <c r="C52" s="1">
         <v>0.66666666666666596</v>
       </c>
-      <c r="D52" s="2">
-        <v>4</v>
-      </c>
-      <c r="E52" s="2">
+      <c r="D52" s="1">
+        <v>4</v>
+      </c>
+      <c r="E52" s="1">
         <v>75</v>
       </c>
-      <c r="F52" s="2">
+      <c r="F52" s="1">
         <v>5.0632911392405E-2</v>
       </c>
-      <c r="G52" s="2">
+      <c r="G52" s="1">
         <v>0.561522678679932</v>
       </c>
     </row>

</xml_diff>